<commit_message>
modified export csv format
</commit_message>
<xml_diff>
--- a/ra_exploer/examples/LTS 智慧資料庫.xlsx
+++ b/ra_exploer/examples/LTS 智慧資料庫.xlsx
@@ -10,12 +10,15 @@
     <sheet name="Milstone" sheetId="1" r:id="rId1"/>
     <sheet name="LTS" sheetId="7" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="125725" calcMode="manual"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">LTS!$A$2:$L$35</definedName>
+  </definedNames>
+  <calcPr calcId="125725" iterate="1" iterateCount="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="37">
   <si>
     <t>PI</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -59,7 +62,7 @@
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -191,7 +194,7 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF3333FF"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -214,7 +217,7 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF3333FF"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -237,7 +240,7 @@
       <rPr>
         <sz val="12"/>
         <color rgb="FF3333FF"/>
-        <rFont val="新細明體"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -260,6 +263,12 @@
   <si>
     <t>Y2</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>Bulk LTS.xlsx</t>
   </si>
 </sst>
 </file>
@@ -270,13 +279,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -289,7 +298,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -323,7 +332,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF3333FF"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -438,10 +447,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -494,7 +503,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -538,7 +547,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -565,13 +574,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>94295</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>28257</xdr:rowOff>
@@ -603,13 +612,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>437238</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>113500</xdr:rowOff>
@@ -641,13 +650,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>24</xdr:col>
+      <xdr:col>25</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>38</xdr:col>
+      <xdr:col>39</xdr:col>
       <xdr:colOff>198800</xdr:colOff>
       <xdr:row>18</xdr:row>
       <xdr:rowOff>18576</xdr:rowOff>
@@ -971,7 +980,7 @@
       <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -981,1238 +990,1339 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="14" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5" style="1" customWidth="1"/>
-    <col min="6" max="6" width="21.375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.75" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="16.625" style="16" customWidth="1"/>
-    <col min="11" max="11" width="79.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="9" style="1"/>
+    <col min="2" max="2" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1"/>
+    <col min="4" max="4" width="14" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="19.75" style="1" customWidth="1"/>
+    <col min="9" max="9" width="16.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="16.625" style="16" customWidth="1"/>
+    <col min="12" max="12" width="79.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:12">
+      <c r="B1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="18" t="s">
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="K1" s="17" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="3" customFormat="1" ht="33">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:12" s="3" customFormat="1" ht="47.25">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="J2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="K2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="7" t="s">
+      <c r="L2" s="7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="3" customFormat="1">
-      <c r="A3" s="8" t="s">
-        <v>5</v>
+    <row r="3" spans="1:12" s="3" customFormat="1">
+      <c r="A3" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="9" t="s">
-        <v>8</v>
+      <c r="D3" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="11">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H3" s="9">
+      <c r="G3" s="11">
+        <v>1</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9">
         <v>-20</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="J3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="3" customFormat="1">
-      <c r="A4" s="8" t="s">
-        <v>5</v>
+      <c r="K3" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="3" customFormat="1">
+      <c r="A4" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>8</v>
+      <c r="D4" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="11">
-        <v>1</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H4" s="9">
+      <c r="G4" s="11">
+        <v>1</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I4" s="9">
         <v>-30</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="J4" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="3" customFormat="1">
-      <c r="A5" s="8" t="s">
-        <v>5</v>
+      <c r="K4" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" s="3" customFormat="1">
+      <c r="A5" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="9" t="s">
-        <v>8</v>
+      <c r="D5" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="11">
-        <v>1</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="9">
+      <c r="G5" s="11">
+        <v>1</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
         <v>-40</v>
       </c>
-      <c r="I5" s="14">
+      <c r="J5" s="14">
         <v>7</v>
       </c>
-      <c r="J5" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11">
-      <c r="A6" s="8" t="s">
-        <v>5</v>
+      <c r="K5" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="11">
-        <v>1</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H6" s="9">
+      <c r="G6" s="11">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9">
         <v>-30</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="J6" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="K6" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="8" t="s">
-        <v>5</v>
+      <c r="L6" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E7" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="11">
-        <v>1</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" s="9">
+      <c r="G7" s="11">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
         <v>-40</v>
       </c>
-      <c r="I7" s="14">
-        <v>8</v>
-      </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="14">
+        <v>8</v>
+      </c>
+      <c r="K7" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="K7" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="A8" s="8" t="s">
-        <v>5</v>
+      <c r="L7" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E8" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="11">
-        <v>1</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H8" s="9">
+      <c r="G8" s="11">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
         <v>-50</v>
       </c>
-      <c r="I8" s="14">
+      <c r="J8" s="14">
         <v>3</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="K8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="A9" s="8" t="s">
+      <c r="L8" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="C9" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>8</v>
+      <c r="D9" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E9" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="11">
-        <v>1</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H9" s="9">
+      <c r="G9" s="11">
+        <v>1</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
         <v>-20</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="J9" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="A10" s="8" t="s">
+      <c r="K9" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="C10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>8</v>
+      <c r="D10" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="11">
-        <v>1</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H10" s="9">
+      <c r="G10" s="11">
+        <v>1</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="9">
         <v>-30</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="J10" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K10" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="A11" s="8" t="s">
+      <c r="K10" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="A11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="C11" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>8</v>
+      <c r="D11" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E11" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="11">
-        <v>1</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H11" s="9">
+      <c r="G11" s="11">
+        <v>1</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="9">
         <v>-40</v>
       </c>
-      <c r="I11" s="14">
-        <v>5</v>
-      </c>
-      <c r="J11" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K11" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="A12" s="8" t="s">
+      <c r="J11" s="14">
+        <v>5</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="C12" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E12" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="11">
-        <v>1</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H12" s="9">
+      <c r="G12" s="11">
+        <v>1</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="9">
         <v>-30</v>
       </c>
-      <c r="I12" s="14" t="s">
+      <c r="J12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K12" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="A13" s="8" t="s">
+      <c r="K12" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="C13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E13" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="11">
-        <v>1</v>
-      </c>
-      <c r="G13" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="9">
+      <c r="G13" s="11">
+        <v>1</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="9">
         <v>-40</v>
       </c>
-      <c r="I13" s="14">
-        <v>8</v>
-      </c>
-      <c r="J13" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K13" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="A14" s="8" t="s">
+      <c r="J13" s="14">
+        <v>8</v>
+      </c>
+      <c r="K13" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E14" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F14" s="11">
-        <v>1</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" s="9">
+      <c r="G14" s="11">
+        <v>1</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="9">
         <v>-50</v>
       </c>
-      <c r="I14" s="14">
+      <c r="J14" s="14">
         <v>2</v>
       </c>
-      <c r="J14" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K14" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="A15" s="8" t="s">
-        <v>5</v>
+      <c r="K14" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L14" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>8</v>
+      <c r="D15" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E15" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="11">
+      <c r="G15" s="11">
         <v>0.95</v>
       </c>
-      <c r="G15" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="9">
+      <c r="H15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="9">
         <v>-20</v>
       </c>
-      <c r="I15" s="14" t="s">
+      <c r="J15" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K15" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="A16" s="8" t="s">
-        <v>5</v>
+      <c r="K15" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>8</v>
+      <c r="D16" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="11">
+      <c r="G16" s="11">
         <v>0.95</v>
       </c>
-      <c r="G16" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="9">
+      <c r="H16" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="9">
         <v>-30</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="J16" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J16" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K16" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11">
-      <c r="A17" s="8" t="s">
-        <v>5</v>
+      <c r="K16" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>8</v>
+      <c r="D17" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E17" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="11">
+      <c r="G17" s="11">
         <v>0.95</v>
       </c>
-      <c r="G17" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="9">
+      <c r="H17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I17" s="9">
         <v>-40</v>
       </c>
-      <c r="I17" s="14">
+      <c r="J17" s="14">
         <v>3</v>
       </c>
-      <c r="J17" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11">
-      <c r="A18" s="8" t="s">
-        <v>5</v>
+      <c r="K17" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E18" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="11">
+      <c r="G18" s="11">
         <v>0.95</v>
       </c>
-      <c r="G18" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="9">
+      <c r="H18" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="9">
         <v>-30</v>
       </c>
-      <c r="I18" s="14" t="s">
+      <c r="J18" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="14" t="s">
+      <c r="K18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="K18" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11">
-      <c r="A19" s="8" t="s">
-        <v>5</v>
+      <c r="L18" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B19" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="D19" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E19" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="11">
+      <c r="G19" s="11">
         <v>0.95</v>
       </c>
-      <c r="G19" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="9">
+      <c r="H19" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I19" s="9">
         <v>-40</v>
       </c>
-      <c r="I19" s="14" t="s">
+      <c r="J19" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J19" s="14" t="s">
+      <c r="K19" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="K19" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" s="8" t="s">
-        <v>5</v>
+      <c r="L19" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B20" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="D20" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D20" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E20" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F20" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="11">
+      <c r="G20" s="11">
         <v>0.95</v>
       </c>
-      <c r="G20" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="9">
         <v>-50</v>
       </c>
-      <c r="I20" s="14">
+      <c r="J20" s="14">
         <v>2</v>
       </c>
-      <c r="J20" s="14" t="s">
+      <c r="K20" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="K20" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" s="8" t="s">
-        <v>5</v>
+      <c r="L20" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="9" t="s">
-        <v>8</v>
+      <c r="D21" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E21" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="11">
+      <c r="G21" s="11">
         <v>0.9</v>
       </c>
-      <c r="G21" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="9">
+      <c r="H21" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" s="9">
         <v>-20</v>
       </c>
-      <c r="I21" s="14" t="s">
+      <c r="J21" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J21" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K21" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11">
-      <c r="A22" s="8" t="s">
-        <v>5</v>
+      <c r="K21" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L21" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>8</v>
+      <c r="D22" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E22" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="11">
+      <c r="G22" s="11">
         <v>0.9</v>
       </c>
-      <c r="G22" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="9">
+      <c r="H22" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="9">
         <v>-30</v>
       </c>
-      <c r="I22" s="14" t="s">
+      <c r="J22" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J22" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K22" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11">
-      <c r="A23" s="8" t="s">
-        <v>5</v>
+      <c r="K22" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L22" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>8</v>
+      <c r="D23" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E23" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="11">
+      <c r="G23" s="11">
         <v>0.9</v>
       </c>
-      <c r="G23" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" s="9">
+      <c r="H23" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="9">
         <v>-40</v>
       </c>
-      <c r="I23" s="14">
-        <v>5</v>
-      </c>
-      <c r="J23" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K23" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11">
-      <c r="A24" s="8" t="s">
-        <v>5</v>
+      <c r="J23" s="14">
+        <v>5</v>
+      </c>
+      <c r="K23" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L23" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B24" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="D24" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E24" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F24" s="11">
+      <c r="G24" s="11">
         <v>0.9</v>
       </c>
-      <c r="G24" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H24" s="9">
+      <c r="H24" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I24" s="9">
         <v>-30</v>
       </c>
-      <c r="I24" s="14" t="s">
+      <c r="J24" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J24" s="14" t="s">
+      <c r="K24" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="K24" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11">
-      <c r="A25" s="8" t="s">
-        <v>5</v>
+      <c r="L24" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B25" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D25" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E25" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="11">
+      <c r="G25" s="11">
         <v>0.9</v>
       </c>
-      <c r="G25" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="9">
+      <c r="H25" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I25" s="9">
         <v>-40</v>
       </c>
-      <c r="I25" s="14" t="s">
+      <c r="J25" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J25" s="14" t="s">
+      <c r="K25" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="K25" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11">
-      <c r="A26" s="8" t="s">
-        <v>5</v>
+      <c r="L25" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B26" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="D26" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E26" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="11">
+      <c r="G26" s="11">
         <v>0.9</v>
       </c>
-      <c r="G26" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H26" s="9">
+      <c r="H26" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" s="9">
         <v>-50</v>
       </c>
-      <c r="I26" s="14">
+      <c r="J26" s="14">
         <v>2</v>
       </c>
-      <c r="J26" s="14" t="s">
+      <c r="K26" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="K26" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11">
-      <c r="A27" s="8" t="s">
-        <v>5</v>
+      <c r="L26" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C27" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>8</v>
+      <c r="D27" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E27" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="11">
+      <c r="G27" s="11">
         <v>0.85</v>
       </c>
-      <c r="G27" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" s="9">
+      <c r="H27" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" s="9">
         <v>-20</v>
       </c>
-      <c r="I27" s="14" t="s">
+      <c r="J27" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J27" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K27" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11">
-      <c r="A28" s="8" t="s">
-        <v>5</v>
+      <c r="K27" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L27" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D28" s="9" t="s">
-        <v>8</v>
+      <c r="D28" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E28" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="11">
+      <c r="G28" s="11">
         <v>0.85</v>
       </c>
-      <c r="G28" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" s="9">
+      <c r="H28" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" s="9">
         <v>-30</v>
       </c>
-      <c r="I28" s="14" t="s">
+      <c r="J28" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J28" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K28" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11">
-      <c r="A29" s="8" t="s">
-        <v>5</v>
+      <c r="K28" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L28" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C29" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="9" t="s">
-        <v>8</v>
+      <c r="D29" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E29" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="11">
+      <c r="G29" s="11">
         <v>0.85</v>
       </c>
-      <c r="G29" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" s="9">
+      <c r="H29" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I29" s="9">
         <v>-40</v>
       </c>
-      <c r="I29" s="14">
-        <v>5</v>
-      </c>
-      <c r="J29" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="K29" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11">
-      <c r="A30" s="8" t="s">
-        <v>5</v>
+      <c r="J29" s="14">
+        <v>5</v>
+      </c>
+      <c r="K29" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="L29" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B30" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D30" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E30" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F30" s="11">
+      <c r="G30" s="11">
         <v>0.85</v>
       </c>
-      <c r="G30" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" s="9">
+      <c r="H30" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30" s="9">
         <v>-30</v>
       </c>
-      <c r="I30" s="14" t="s">
+      <c r="J30" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="J30" s="14" t="s">
+      <c r="K30" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="K30" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11">
-      <c r="A31" s="8" t="s">
-        <v>5</v>
+      <c r="L30" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B31" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="D31" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E31" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F31" s="11">
+      <c r="G31" s="11">
         <v>0.85</v>
       </c>
-      <c r="G31" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="9">
+      <c r="H31" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" s="9">
         <v>-40</v>
       </c>
-      <c r="I31" s="14" t="s">
+      <c r="J31" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="J31" s="14" t="s">
+      <c r="K31" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="K31" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11">
-      <c r="A32" s="8" t="s">
-        <v>5</v>
+      <c r="L31" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B32" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="D32" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="9" t="s">
-        <v>8</v>
-      </c>
       <c r="E32" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F32" s="11">
+      <c r="G32" s="11">
         <v>0.85</v>
       </c>
-      <c r="G32" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" s="9">
+      <c r="H32" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I32" s="9">
         <v>-50</v>
       </c>
-      <c r="I32" s="14">
+      <c r="J32" s="14">
         <v>2</v>
       </c>
-      <c r="J32" s="14" t="s">
+      <c r="K32" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="K32" s="10" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11">
-      <c r="A33" s="8" t="s">
+      <c r="L32" s="10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B33" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="C33" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D33" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="E33" s="8" t="s">
+      <c r="F33" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F33" s="11">
-        <v>1</v>
-      </c>
-      <c r="G33" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" s="8">
+      <c r="G33" s="11">
+        <v>1</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I33" s="8">
         <v>-30</v>
       </c>
-      <c r="I33" s="15">
+      <c r="J33" s="15">
         <v>10</v>
       </c>
-      <c r="J33" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="K33" s="12" t="s">
+      <c r="K33" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L33" s="12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G34" s="11">
+        <v>1</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I34" s="8">
+        <v>-30</v>
+      </c>
+      <c r="J34" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="K34" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L34" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G35" s="11">
+        <v>1</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" s="8">
+        <v>-30</v>
+      </c>
+      <c r="J35" s="15">
+        <v>12</v>
+      </c>
+      <c r="K35" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="L35" s="12" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
-      <c r="A34" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F34" s="11">
-        <v>1</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H34" s="8">
-        <v>-30</v>
-      </c>
-      <c r="I34" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="J34" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="K34" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="F35" s="11">
-        <v>1</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="8">
-        <v>-30</v>
-      </c>
-      <c r="I35" s="15">
-        <v>12</v>
-      </c>
-      <c r="J35" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="K35" s="12" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="A2:L35"/>
   <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="B1:I1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>